<commit_message>
Just finished the bad ass Base API local Grid Cloud
</commit_message>
<xml_diff>
--- a/DEMOQA/src/test/Resources/TestData_RegistraionForm/DemoQA_RegistrationPage.xlsx
+++ b/DEMOQA/src/test/Resources/TestData_RegistraionForm/DemoQA_RegistrationPage.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sami/Desktop/SeleniumBootCamp/DEMOQA/src/test/Resources/TestData_RegistraionForm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sami/IdeaProjects/SeleniumBootCamp/DEMOQA/src/test/Resources/TestData_RegistraionForm/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="1140" windowWidth="13980" windowHeight="10960" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>TestCases</t>
   </si>
@@ -36,83 +36,103 @@
     <t>Y</t>
   </si>
   <si>
-    <t>OpenAccountTest</t>
-  </si>
-  <si>
     <t>firstname</t>
   </si>
   <si>
     <t>lastname</t>
   </si>
   <si>
-    <t>postcode</t>
-  </si>
-  <si>
-    <t>browser</t>
-  </si>
-  <si>
-    <t>Raman</t>
-  </si>
-  <si>
-    <t>Arora</t>
-  </si>
-  <si>
-    <t>A234324</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>D53434</t>
-  </si>
-  <si>
-    <t>firefox</t>
-  </si>
-  <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>customer</t>
-  </si>
-  <si>
-    <t>currency</t>
-  </si>
-  <si>
-    <t>Harry Potter</t>
-  </si>
-  <si>
-    <t>Rupee</t>
-  </si>
-  <si>
-    <t>Ron Weasly</t>
-  </si>
-  <si>
-    <t>Dollar</t>
-  </si>
-  <si>
-    <t>Hermoine Granger</t>
-  </si>
-  <si>
-    <t>Pound</t>
-  </si>
-  <si>
-    <t>Registration001</t>
+    <t>RegistrationDemoExcel</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>sami</t>
+  </si>
+  <si>
+    <t>sabir</t>
+  </si>
+  <si>
+    <t>571 550 3399</t>
+  </si>
+  <si>
+    <t>sami212</t>
+  </si>
+  <si>
+    <t>samisabir212@gmail.com</t>
+  </si>
+  <si>
+    <t>secretpassword</t>
+  </si>
+  <si>
+    <t>veronika</t>
+  </si>
+  <si>
+    <t>veronika212</t>
+  </si>
+  <si>
+    <t>veronika92@gmail.com</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>not supposed to run</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>test212</t>
+  </si>
+  <si>
+    <t>test212@gmail.com</t>
+  </si>
+  <si>
+    <t>confirm_password</t>
+  </si>
+  <si>
+    <t>phone_number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,13 +155,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -417,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -438,17 +480,9 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -459,150 +493,150 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="18.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="18.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>25</v>
-      </c>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="H5" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="K5" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="F5" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>